<commit_message>
Added to Recipe_List and fixed package.json so it can start the server
</commit_message>
<xml_diff>
--- a/Recipe_List.xlsx
+++ b/Recipe_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natew\Desktop\Fall 2016\CS_291\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natew\Documents\GitHub\Recipe-Repository-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>MEXICAN RECIPES</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Mixing bowl</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Serves 3-4</t>
   </si>
 </sst>
 </file>
@@ -664,8 +670,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1134,7 +1140,9 @@
       <c r="B72" s="1"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="B73" s="1"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1335,7 +1343,9 @@
       <c r="A102" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final push for the night
</commit_message>
<xml_diff>
--- a/Recipe_List.xlsx
+++ b/Recipe_List.xlsx
@@ -668,10 +668,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,650 +700,586 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
+      <c r="A50" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="A56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="A57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
+      <c r="A58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" s="2"/>
+      <c r="A59" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="1"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" s="2"/>
+      <c r="A60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" s="2"/>
+      <c r="A61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+      <c r="A62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="2"/>
+      <c r="A63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>69</v>
+      <c r="A64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>70</v>
+      <c r="A65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>71</v>
+      <c r="A66" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>72</v>
+      <c r="A68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B73" s="1"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B75" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B77" s="1"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B79" s="1"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B80" s="1"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B81" s="1"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B102" s="1" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>